<commit_message>
Updated inventory Related test case Added Build.xml File Created Test plan -Happy path -Inventory
</commit_message>
<xml_diff>
--- a/templates/LOCAdd.xlsx
+++ b/templates/LOCAdd.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9FC695-CFE8-4E9A-A1AE-54939C844277}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5331F6F-81A8-4A72-B9EC-27C466FF1007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Location Add" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
   <si>
     <t>OH (On Hand Loc)</t>
   </si>
@@ -115,6 +116,76 @@
   </si>
   <si>
     <t>NN1 (non nettable)</t>
+  </si>
+  <si>
+    <t>100 Home Project</t>
+  </si>
+  <si>
+    <t>LT-1</t>
+  </si>
+  <si>
+    <t>Lot and serial track</t>
+  </si>
+  <si>
+    <t>Serial track</t>
+  </si>
+  <si>
+    <t>no track</t>
+  </si>
+  <si>
+    <t>Lot track</t>
+  </si>
+  <si>
+    <t>1001 (100 Test)</t>
+  </si>
+  <si>
+    <t>multidiv Serial track</t>
+  </si>
+  <si>
+    <t>multidiv no track</t>
+  </si>
+  <si>
+    <t>multidiv LOT</t>
+  </si>
+  <si>
+    <t>multidiv serial (Lot and serial track)</t>
+  </si>
+  <si>
+    <t>LT-2</t>
+  </si>
+  <si>
+    <t>BKF1 (Backflush)</t>
+  </si>
+  <si>
+    <t>INSP (Inspection location)</t>
+  </si>
+  <si>
+    <t>To Con Loc</t>
+  </si>
+  <si>
+    <t>To Insp Loc</t>
+  </si>
+  <si>
+    <t>To BKFL LOC</t>
+  </si>
+  <si>
+    <t>To NN Loc</t>
+  </si>
+  <si>
+    <t>Provar-501
+Provar-502
+Provar-503
+Provar-504
+Provar-505
+Provar-506</t>
+  </si>
+  <si>
+    <t>Provar-601
+Provar-602
+Provar-603
+Provar-604
+Provar-605
+Provar-606</t>
   </si>
 </sst>
 </file>
@@ -156,10 +227,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,35 +514,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="58.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="2">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="58.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="2">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="58.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="2">
+        <v>44328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="58.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>30</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="2">
+        <v>44328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB06652-2BC0-42CE-AADC-40B9F44B2386}">
+  <dimension ref="A1:U6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -659,11 +1076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code optimization-location to location transfer to existing location fixed issue related to reading serial numbers
</commit_message>
<xml_diff>
--- a/templates/LOCAdd.xlsx
+++ b/templates/LOCAdd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C2C462-4AF4-459A-B3ED-E847864A0BCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00867D4-BC86-48BF-A32A-B23325EAC958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,7 +176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +189,13 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,13 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +507,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="A9:XFD9"/>
+      <selection activeCell="A2" sqref="A2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +521,7 @@
     <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
@@ -556,7 +562,7 @@
       <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="K1" t="s">
@@ -591,268 +597,267 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="3">
+        <v>44328</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="3">
+        <v>45058</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>40</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I6" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J6" s="3">
         <v>44693</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D7" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="2">
-        <v>44328</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D8" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="3">
-        <v>6</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D9" t="s">
         <v>0</v>
-      </c>
-      <c r="E7">
-        <v>30</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>40</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="2">
-        <v>44328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E9">
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="3">
+        <v>44328</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
+      <c r="D10" t="s">
+        <v>43</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
+      <c r="D11" t="s">
+        <v>29</v>
       </c>
       <c r="E11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
+      <c r="D12" t="s">
+        <v>42</v>
       </c>
       <c r="E12">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="H13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="2">
-        <v>45058</v>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code for RSTK-8093_RSTK-8109_RSTK-8939 and modified templates
</commit_message>
<xml_diff>
--- a/templates/LOCAdd.xlsx
+++ b/templates/LOCAdd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439D635E-396F-4D6C-A0C1-6346B22B5EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C10B45E-DBE2-4874-BC9D-287EAAF796E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="66">
   <si>
     <t>OH (On Hand Loc)</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>Lot track-To OH loc-backdated</t>
+  </si>
+  <si>
+    <t>1019 (100 MS-project)</t>
+  </si>
+  <si>
+    <t>Pro-1</t>
+  </si>
+  <si>
+    <t>LT3</t>
+  </si>
+  <si>
+    <t>LT1</t>
   </si>
 </sst>
 </file>
@@ -552,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J6"/>
+      <selection activeCell="B3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,25 +576,26 @@
     <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -596,55 +609,58 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -657,23 +673,23 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>44353</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>61</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -686,20 +702,20 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1100</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>56</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -712,20 +728,20 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1200</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>55</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -738,20 +754,20 @@
       <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1300</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>57</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -764,20 +780,20 @@
       <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1400</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>58</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -790,14 +806,14 @@
       <c r="D7" t="s">
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>15</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -810,14 +826,14 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>16</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -830,14 +846,14 @@
       <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>17</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -850,14 +866,14 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>18</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -870,14 +886,14 @@
       <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -885,26 +901,22 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
-      <c r="E12">
-        <v>20</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="H12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="3">
-        <v>45058</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -915,22 +927,19 @@
         <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J13" s="3">
-        <v>45058</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -941,22 +950,23 @@
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14">
-        <v>22</v>
-      </c>
-      <c r="H14" t="s">
-        <v>47</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="I14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" s="3">
+        <v>45</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -967,22 +977,22 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="F15">
+        <v>21</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="3">
+        <v>46</v>
+      </c>
+      <c r="J15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -990,65 +1000,77 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="3">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="3">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E16">
+      <c r="F18">
         <v>24</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I18" t="s">
         <v>48</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J18" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K18" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>2500</v>
-      </c>
-      <c r="H17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18">
-        <v>2600</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1059,17 +1081,16 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19">
-        <v>2700</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="H19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2500</v>
+      </c>
+      <c r="I19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1077,19 +1098,19 @@
         <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20">
-        <v>2800</v>
-      </c>
-      <c r="H20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <v>2600</v>
+      </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1100,12 +1121,53 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21">
+        <v>2700</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="I21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22">
+        <v>2800</v>
+      </c>
+      <c r="I22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
         <v>38</v>
       </c>
-      <c r="E21">
+      <c r="F23">
         <v>2900</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I23" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1121,7 +1183,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="A1:XFD1048576"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Code For inventory Transactions
</commit_message>
<xml_diff>
--- a/templates/LOCAdd.xlsx
+++ b/templates/LOCAdd.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439D635E-396F-4D6C-A0C1-6346B22B5EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3456C119-03D3-4CC5-8037-65A89BC16C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="65">
   <si>
     <t>OH (On Hand Loc)</t>
   </si>
@@ -212,13 +212,22 @@
   </si>
   <si>
     <t>Lot track-To OH loc-backdated</t>
+  </si>
+  <si>
+    <t>LT_SY1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lot and serial </t>
+  </si>
+  <si>
+    <t>MNK60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +254,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -266,12 +288,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,25 +588,26 @@
     <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -596,84 +621,87 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2" s="3">
-        <v>44353</v>
-      </c>
-      <c r="H2" t="s">
-        <v>61</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="3">
+        <v>63</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="5">
         <v>45058</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -681,25 +709,28 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3">
-        <v>1100</v>
-      </c>
-      <c r="H3" t="s">
-        <v>56</v>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44353</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="3">
+        <v>61</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -710,22 +741,22 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4">
-        <v>1200</v>
-      </c>
-      <c r="H4" t="s">
-        <v>55</v>
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>1100</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="3">
+        <v>56</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -736,22 +767,22 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5">
-        <v>1300</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
+        <v>29</v>
+      </c>
+      <c r="F5">
+        <v>1200</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="3">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -762,42 +793,48 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>1300</v>
+      </c>
+      <c r="I6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="3">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="E6">
+      <c r="F7">
         <v>1400</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I7" t="s">
         <v>58</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J7" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K7" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -808,16 +845,16 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -828,16 +865,16 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -845,19 +882,19 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -865,46 +902,39 @@
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="E11">
+      <c r="F12">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>20</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="H12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="3">
-        <v>45058</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -912,25 +942,26 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>46</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13" s="3"/>
       <c r="I13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J13" s="3">
+        <v>45</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -938,25 +969,25 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14">
-        <v>22</v>
-      </c>
-      <c r="H14" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>21</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" s="3">
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -964,25 +995,25 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
-        <v>49</v>
+        <v>29</v>
+      </c>
+      <c r="F15">
+        <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="3">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -993,42 +1024,48 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="3">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="E16">
+      <c r="F17">
         <v>24</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I17" t="s">
         <v>48</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J17" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K17" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>2500</v>
-      </c>
-      <c r="H17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1036,19 +1073,19 @@
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18">
-        <v>2600</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>2500</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1056,20 +1093,19 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19">
-        <v>2700</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="H19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>2600</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1080,16 +1116,17 @@
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20">
-        <v>2800</v>
-      </c>
-      <c r="H20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="F20">
+        <v>2700</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="I20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1100,13 +1137,38 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <v>2800</v>
+      </c>
+      <c r="I21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
         <v>38</v>
       </c>
-      <c r="E21">
+      <c r="F22">
         <v>2900</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I22" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Data for Inventory Transaction Added Testcase for Regular WO Added Testcase for Rework WO Created callable testcase for Add operation
</commit_message>
<xml_diff>
--- a/templates/LOCAdd.xlsx
+++ b/templates/LOCAdd.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3456C119-03D3-4CC5-8037-65A89BC16C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069F298E-58FF-42D4-A265-58BE1BFB0399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Location Add" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="60">
   <si>
     <t>OH (On Hand Loc)</t>
   </si>
   <si>
-    <t>MS-No track</t>
-  </si>
-  <si>
-    <t>MS-Lot track item</t>
-  </si>
-  <si>
     <t>Item Name</t>
   </si>
   <si>
@@ -94,24 +87,15 @@
     <t>Project</t>
   </si>
   <si>
-    <t>1006 (100 SB Test Proj-01)</t>
-  </si>
-  <si>
     <t>Lot No</t>
   </si>
   <si>
     <t>Lot Expiration Date</t>
   </si>
   <si>
-    <t>6644-6</t>
-  </si>
-  <si>
     <t>10 (Denver)</t>
   </si>
   <si>
-    <t>Test Lot Track</t>
-  </si>
-  <si>
     <t>CON (Consigned)</t>
   </si>
   <si>
@@ -127,15 +111,6 @@
     <t>1001 (100 Test)</t>
   </si>
   <si>
-    <t>multidiv Serial track</t>
-  </si>
-  <si>
-    <t>multidiv no track</t>
-  </si>
-  <si>
-    <t>multidiv LOT</t>
-  </si>
-  <si>
     <t>multidiv serial (Lot and serial track)</t>
   </si>
   <si>
@@ -221,25 +196,28 @@
   </si>
   <si>
     <t>MNK60</t>
+  </si>
+  <si>
+    <t>multidiv LOT (Lot track)</t>
+  </si>
+  <si>
+    <t>multidiv Serial track (Serial track)</t>
+  </si>
+  <si>
+    <t>multidiv no track (no track)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="7"/>
@@ -288,14 +266,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,25 +552,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F7" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
@@ -609,340 +585,340 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44353</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="K2" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F3">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="3">
-        <v>44353</v>
+        <v>1100</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="3">
+        <v>29</v>
+      </c>
+      <c r="K3" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="3">
+        <v>51</v>
+      </c>
+      <c r="K4" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F5">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="3">
+        <v>52</v>
+      </c>
+      <c r="K5" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>1400</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6">
-        <v>1300</v>
-      </c>
-      <c r="I6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="K6" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1400</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="3">
-        <v>45058</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F11">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12">
-        <v>19</v>
-      </c>
       <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
         <v>54</v>
+      </c>
+      <c r="K12" s="3">
+        <v>45058</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -950,130 +926,130 @@
       <c r="F13">
         <v>20</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="1"/>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="3">
+        <v>26</v>
+      </c>
+      <c r="K13" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>21</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="3">
+        <v>29</v>
+      </c>
+      <c r="K14" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F15">
         <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
-      </c>
-      <c r="K15" s="3">
+        <v>51</v>
+      </c>
+      <c r="K15" s="1">
         <v>45058</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F16">
         <v>23</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="3">
+        <v>52</v>
+      </c>
+      <c r="K16" s="1">
         <v>45058</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
         <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
       </c>
       <c r="F17">
         <v>24</v>
       </c>
       <c r="I17" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
-      </c>
-      <c r="K17" s="3">
+        <v>26</v>
+      </c>
+      <c r="K17" s="1">
         <v>45058</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -1082,302 +1058,93 @@
         <v>2500</v>
       </c>
       <c r="I18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F19">
         <v>2600</v>
       </c>
       <c r="I19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F20">
         <v>2700</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="1"/>
       <c r="I20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F21">
         <v>2800</v>
       </c>
       <c r="I21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
         <v>30</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
       </c>
       <c r="F22">
         <v>2900</v>
       </c>
       <c r="I22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M24">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB06652-2BC0-42CE-AADC-40B9F44B2386}">
-  <dimension ref="A1:U6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1221</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2">
-        <v>44311</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2">
-        <v>44311</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1221</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2">
-        <v>44311</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3" s="2">
-        <v>44311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1221</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2">
-        <v>44311</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4" s="2">
-        <v>44311</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>213</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>121</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added SYDATA WO Transactions Added Test Plan
</commit_message>
<xml_diff>
--- a/templates/LOCAdd.xlsx
+++ b/templates/LOCAdd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\rsqasampleproj\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069F298E-58FF-42D4-A265-58BE1BFB0399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62823B2-E660-437D-8EB2-71C627420A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Location Add" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="A2:XFD7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>